<commit_message>
Make test with the lastest V7 version
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/B1_Model_Structure.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/B1_Model_Structure.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{838D6DA1-B740-476B-8C62-57EBF32FF73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EF172DB-2227-4B38-B172-BE178C347DD2}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{838D6DA1-B740-476B-8C62-57EBF32FF73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07790577-6CD0-4302-AA51-A99AF909A742}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
     <sheet name="sector" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">sector!$A$1:$C$302</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">sector!$A$1:$C$304</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sets!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="632">
   <si>
     <t>set</t>
   </si>
@@ -1925,13 +1925,19 @@
   </si>
   <si>
     <t>CO2e_DE</t>
+  </si>
+  <si>
+    <t>TRTAXELE</t>
+  </si>
+  <si>
+    <t>TRSUVELE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1946,6 +1952,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2007,7 +2019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2017,6 +2029,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2297,13 +2310,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L304"/>
+  <dimension ref="A1:L306"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C210" sqref="C210:C292"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -2404,7 +2417,7 @@
       </c>
       <c r="C3">
         <f>+COUNTA(C4:C1048576)</f>
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
@@ -4265,17 +4278,17 @@
     </row>
     <row r="216" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C216" t="s">
-        <v>282</v>
+        <v>180</v>
       </c>
     </row>
     <row r="217" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C217" t="s">
-        <v>177</v>
+        <v>282</v>
       </c>
     </row>
     <row r="218" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C218" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="219" spans="3:3" x14ac:dyDescent="0.3">
@@ -4395,316 +4408,326 @@
     </row>
     <row r="242" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C242" t="s">
-        <v>198</v>
+        <v>630</v>
       </c>
     </row>
     <row r="243" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C243" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="244" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C244" t="s">
-        <v>486</v>
+        <v>199</v>
       </c>
     </row>
     <row r="245" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C245" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="246" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C246" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="247" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C247" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="248" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C248" t="s">
-        <v>271</v>
+        <v>631</v>
       </c>
     </row>
     <row r="249" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C249" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="250" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C250" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="251" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C251" t="s">
-        <v>273</v>
+        <v>490</v>
       </c>
     </row>
     <row r="252" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C252" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="253" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C253" t="s">
-        <v>491</v>
+        <v>273</v>
       </c>
     </row>
     <row r="254" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C254" t="s">
-        <v>492</v>
+        <v>274</v>
       </c>
     </row>
     <row r="255" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C255" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="256" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C256" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="257" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C257" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="258" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C258" t="s">
-        <v>268</v>
+        <v>494</v>
       </c>
     </row>
     <row r="259" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C259" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="260" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C260" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="261" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C261" t="s">
-        <v>270</v>
+        <v>496</v>
       </c>
     </row>
     <row r="262" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C262" t="s">
-        <v>240</v>
+        <v>269</v>
       </c>
     </row>
     <row r="263" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C263" t="s">
-        <v>200</v>
+        <v>270</v>
       </c>
     </row>
     <row r="264" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C264" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
     </row>
     <row r="265" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C265" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="266" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C266" t="s">
-        <v>497</v>
+        <v>201</v>
       </c>
     </row>
     <row r="267" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C267" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="268" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C268" t="s">
-        <v>204</v>
+        <v>497</v>
       </c>
     </row>
     <row r="269" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C269" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="270" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C270" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
     </row>
     <row r="271" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C271" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="272" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C272" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
     </row>
     <row r="273" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C273" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="274" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C274" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="275" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C275" t="s">
-        <v>498</v>
+        <v>208</v>
       </c>
     </row>
     <row r="276" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C276" t="s">
-        <v>242</v>
+        <v>209</v>
       </c>
     </row>
     <row r="277" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C277" t="s">
-        <v>243</v>
+        <v>498</v>
       </c>
     </row>
     <row r="278" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C278" t="s">
-        <v>499</v>
+        <v>242</v>
       </c>
     </row>
     <row r="279" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C279" t="s">
-        <v>122</v>
+        <v>243</v>
       </c>
     </row>
     <row r="280" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C280" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="281" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C281" t="s">
-        <v>277</v>
+        <v>122</v>
       </c>
     </row>
     <row r="282" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C282" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="283" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C283" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="284" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C284" t="s">
-        <v>244</v>
+        <v>501</v>
       </c>
     </row>
     <row r="285" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C285" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
     </row>
     <row r="286" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C286" t="s">
-        <v>210</v>
+        <v>244</v>
       </c>
     </row>
     <row r="287" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C287" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="288" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C288" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
     </row>
     <row r="289" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C289" t="s">
-        <v>266</v>
+        <v>124</v>
       </c>
     </row>
     <row r="290" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C290" t="s">
-        <v>267</v>
+        <v>125</v>
       </c>
     </row>
     <row r="291" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C291" t="s">
-        <v>605</v>
+        <v>266</v>
       </c>
     </row>
     <row r="292" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C292" t="s">
-        <v>606</v>
+        <v>267</v>
       </c>
     </row>
     <row r="293" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C293" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="294" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C294" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="295" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C295" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="296" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C296" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="297" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C297" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
     </row>
     <row r="298" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C298" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
     </row>
     <row r="299" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C299" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="300" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C300" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="301" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C301" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="302" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C302" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="303" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C303" s="2" t="s">
-        <v>623</v>
+      <c r="C303" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="304" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C304" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="305" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C305" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="306" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C306" t="s">
         <v>624</v>
       </c>
     </row>
@@ -4721,7 +4744,7 @@
       <selection activeCell="AE3" sqref="B3:AE3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" customWidth="1"/>
@@ -5290,7 +5313,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -6129,11 +6152,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B380EC-F6E5-4369-BC41-BC40A47B4895}">
-  <dimension ref="A1:C302"/>
+  <dimension ref="A1:C304"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="F292" sqref="F292"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
@@ -8440,7 +8465,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A210" s="4" t="s">
+      <c r="A210" s="9" t="s">
         <v>170</v>
       </c>
       <c r="B210" s="4" t="s">
@@ -8451,7 +8476,7 @@
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211" s="4" t="s">
+      <c r="A211" s="9" t="s">
         <v>171</v>
       </c>
       <c r="B211" s="4" t="s">
@@ -8462,7 +8487,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A212" s="4" t="s">
+      <c r="A212" s="9" t="s">
         <v>173</v>
       </c>
       <c r="B212" s="4" t="s">
@@ -8473,7 +8498,7 @@
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A213" s="4" t="s">
+      <c r="A213" s="9" t="s">
         <v>175</v>
       </c>
       <c r="B213" s="4" t="s">
@@ -8484,7 +8509,7 @@
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A214" s="4" t="s">
+      <c r="A214" s="9" t="s">
         <v>474</v>
       </c>
       <c r="B214" s="4" t="s">
@@ -8495,7 +8520,7 @@
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A215" s="4" t="s">
+      <c r="A215" s="9" t="s">
         <v>178</v>
       </c>
       <c r="B215" s="4" t="s">
@@ -8506,31 +8531,31 @@
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A216" s="4" t="s">
+      <c r="A216" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="B216" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C216" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A217" s="4" t="s">
+      <c r="B217" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B217" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C217" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A218" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="B218" s="4" t="s">
         <v>627</v>
       </c>
@@ -8539,7 +8564,7 @@
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A219" s="4" t="s">
+      <c r="A219" s="9" t="s">
         <v>475</v>
       </c>
       <c r="B219" s="4" t="s">
@@ -8550,7 +8575,7 @@
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A220" s="4" t="s">
+      <c r="A220" s="9" t="s">
         <v>476</v>
       </c>
       <c r="B220" s="4" t="s">
@@ -8561,7 +8586,7 @@
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A221" s="4" t="s">
+      <c r="A221" s="9" t="s">
         <v>477</v>
       </c>
       <c r="B221" s="4" t="s">
@@ -8572,7 +8597,7 @@
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A222" s="4" t="s">
+      <c r="A222" s="9" t="s">
         <v>478</v>
       </c>
       <c r="B222" s="4" t="s">
@@ -8583,7 +8608,7 @@
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A223" s="4" t="s">
+      <c r="A223" s="9" t="s">
         <v>479</v>
       </c>
       <c r="B223" s="4" t="s">
@@ -8594,7 +8619,7 @@
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A224" s="4" t="s">
+      <c r="A224" s="9" t="s">
         <v>480</v>
       </c>
       <c r="B224" s="4" t="s">
@@ -8605,7 +8630,7 @@
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A225" s="4" t="s">
+      <c r="A225" s="9" t="s">
         <v>184</v>
       </c>
       <c r="B225" s="4" t="s">
@@ -8616,7 +8641,7 @@
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A226" s="4" t="s">
+      <c r="A226" s="9" t="s">
         <v>185</v>
       </c>
       <c r="B226" s="4" t="s">
@@ -8627,7 +8652,7 @@
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A227" s="4" t="s">
+      <c r="A227" s="9" t="s">
         <v>481</v>
       </c>
       <c r="B227" s="4" t="s">
@@ -8638,7 +8663,7 @@
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A228" s="4" t="s">
+      <c r="A228" s="9" t="s">
         <v>186</v>
       </c>
       <c r="B228" s="4" t="s">
@@ -8649,7 +8674,7 @@
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A229" s="4" t="s">
+      <c r="A229" s="9" t="s">
         <v>482</v>
       </c>
       <c r="B229" s="4" t="s">
@@ -8660,7 +8685,7 @@
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A230" s="4" t="s">
+      <c r="A230" s="9" t="s">
         <v>188</v>
       </c>
       <c r="B230" s="4" t="s">
@@ -8671,7 +8696,7 @@
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A231" s="4" t="s">
+      <c r="A231" s="9" t="s">
         <v>189</v>
       </c>
       <c r="B231" s="4" t="s">
@@ -8682,7 +8707,7 @@
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A232" s="4" t="s">
+      <c r="A232" s="9" t="s">
         <v>190</v>
       </c>
       <c r="B232" s="4" t="s">
@@ -8693,7 +8718,7 @@
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A233" s="4" t="s">
+      <c r="A233" s="9" t="s">
         <v>192</v>
       </c>
       <c r="B233" s="4" t="s">
@@ -8704,7 +8729,7 @@
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A234" s="4" t="s">
+      <c r="A234" s="9" t="s">
         <v>483</v>
       </c>
       <c r="B234" s="4" t="s">
@@ -8715,7 +8740,7 @@
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A235" s="4" t="s">
+      <c r="A235" s="9" t="s">
         <v>235</v>
       </c>
       <c r="B235" s="4" t="s">
@@ -8726,7 +8751,7 @@
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A236" s="4" t="s">
+      <c r="A236" s="9" t="s">
         <v>236</v>
       </c>
       <c r="B236" s="4" t="s">
@@ -8737,7 +8762,7 @@
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A237" s="4" t="s">
+      <c r="A237" s="9" t="s">
         <v>237</v>
       </c>
       <c r="B237" s="4" t="s">
@@ -8748,7 +8773,7 @@
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A238" s="4" t="s">
+      <c r="A238" s="9" t="s">
         <v>238</v>
       </c>
       <c r="B238" s="4" t="s">
@@ -8759,7 +8784,7 @@
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A239" s="4" t="s">
+      <c r="A239" s="9" t="s">
         <v>239</v>
       </c>
       <c r="B239" s="4" t="s">
@@ -8770,7 +8795,7 @@
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A240" s="4" t="s">
+      <c r="A240" s="9" t="s">
         <v>484</v>
       </c>
       <c r="B240" s="4" t="s">
@@ -8781,7 +8806,7 @@
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A241" s="4" t="s">
+      <c r="A241" s="9" t="s">
         <v>485</v>
       </c>
       <c r="B241" s="4" t="s">
@@ -8792,561 +8817,561 @@
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A242" s="4" t="s">
+      <c r="A242" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C242" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A243" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B242" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C242" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A243" s="4" t="s">
+      <c r="B243" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C243" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A244" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B243" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C243" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A244" s="4" t="s">
+      <c r="B244" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C244" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A245" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="B244" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C244" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A245" s="4" t="s">
+      <c r="B245" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C245" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A246" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="B245" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C245" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A246" s="4" t="s">
+      <c r="B246" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C246" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A247" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="B246" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C246" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A247" s="4" t="s">
+      <c r="B247" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C247" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A248" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="B248" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C248" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A249" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="B247" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C247" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A248" s="4" t="s">
+      <c r="B249" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C249" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A250" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B248" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C248" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A249" s="4" t="s">
+      <c r="B250" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C250" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A251" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="B249" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C249" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A250" s="4" t="s">
+      <c r="B251" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C251" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A252" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="B250" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C250" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A251" s="4" t="s">
+      <c r="B252" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C252" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A253" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B251" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C251" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A252" s="4" t="s">
+      <c r="B253" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C253" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A254" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="B252" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C252" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A253" s="4" t="s">
+      <c r="B254" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C254" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A255" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="B253" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C253" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A254" s="4" t="s">
+      <c r="B255" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C255" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="B254" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C254" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A255" s="4" t="s">
+      <c r="B256" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C256" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" s="9" t="s">
         <v>493</v>
       </c>
-      <c r="B255" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C255" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A256" s="4" t="s">
+      <c r="B257" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C257" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="B256" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C256" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A257" s="4" t="s">
+      <c r="B258" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C258" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A259" s="9" t="s">
         <v>495</v>
       </c>
-      <c r="B257" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C257" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A258" s="4" t="s">
+      <c r="B259" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C259" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A260" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B258" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C258" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A259" s="4" t="s">
+      <c r="B260" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C260" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A261" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="B259" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C259" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A260" s="4" t="s">
+      <c r="B261" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C261" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A262" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B260" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C260" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A261" s="4" t="s">
+      <c r="B262" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C262" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="B261" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C261" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A262" s="4" t="s">
+      <c r="B263" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C263" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="B262" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C262" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A263" s="4" t="s">
+      <c r="B264" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C264" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A265" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="B263" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C263" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A264" s="4" t="s">
+      <c r="B265" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C265" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A266" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B264" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C264" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A265" s="4" t="s">
+      <c r="B266" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C266" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A267" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B265" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C265" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A266" s="4" t="s">
+      <c r="B267" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C267" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A268" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="B266" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C266" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A267" s="4" t="s">
+      <c r="B268" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C268" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A269" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B267" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C267" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A268" s="4" t="s">
+      <c r="B269" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C269" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A270" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B268" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C268" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A269" s="4" t="s">
+      <c r="B270" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C270" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A271" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B269" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C269" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A270" s="4" t="s">
+      <c r="B271" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C271" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A272" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="B270" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C270" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A271" s="4" t="s">
+      <c r="B272" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C272" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A273" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B271" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C271" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A272" s="4" t="s">
+      <c r="B273" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C273" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A274" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B272" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C272" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A273" s="4" t="s">
+      <c r="B274" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C274" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A275" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B273" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C273" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A274" s="4" t="s">
+      <c r="B275" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C275" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A276" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B274" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C274" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A275" s="4" t="s">
+      <c r="B276" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C276" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A277" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="B275" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C275" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A276" s="4" t="s">
+      <c r="B277" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C277" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A278" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="B276" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C276" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A277" s="4" t="s">
+      <c r="B278" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C278" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A279" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B277" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C277" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A278" s="4" t="s">
+      <c r="B279" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C279" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A280" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="B278" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C278" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A279" s="4" t="s">
+      <c r="B280" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C280" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A281" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B279" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C279" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A280" s="4" t="s">
+      <c r="B281" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C281" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A282" s="9" t="s">
         <v>500</v>
       </c>
-      <c r="B280" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C280" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A281" s="4" t="s">
+      <c r="B282" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C282" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A283" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="B281" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C281" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A282" s="4" t="s">
+      <c r="B283" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C283" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A284" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="B282" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C282" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A283" s="4" t="s">
+      <c r="B284" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C284" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A285" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="B283" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C283" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A284" s="4" t="s">
+      <c r="B285" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C285" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A286" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="B284" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C284" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A285" s="4" t="s">
+      <c r="B286" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C286" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A287" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B285" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C285" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A286" s="4" t="s">
+      <c r="B287" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C287" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A288" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="B286" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C286" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A287" s="4" t="s">
+      <c r="B288" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C288" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A289" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B287" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C287" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A288" s="4" t="s">
+      <c r="B289" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C289" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A290" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B288" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C288" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A289" s="4" t="s">
+      <c r="B290" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C290" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A291" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B289" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C289" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A290" s="4" t="s">
+      <c r="B291" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C291" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A292" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B290" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="C290" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A291" s="6" t="s">
-        <v>605</v>
-      </c>
-      <c r="B291" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="C291" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A292" s="6" t="s">
-        <v>606</v>
-      </c>
       <c r="B292" s="4" t="s">
-        <v>615</v>
+        <v>627</v>
       </c>
       <c r="C292" s="4" t="s">
         <v>613</v>
@@ -9354,7 +9379,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" s="6" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B293" s="4" t="s">
         <v>615</v>
@@ -9365,7 +9390,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" s="6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B294" s="4" t="s">
         <v>615</v>
@@ -9375,44 +9400,44 @@
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A295" s="5" t="s">
+      <c r="A295" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="B295" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C295" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A296" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B296" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C296" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A297" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="B295" s="4" t="s">
+      <c r="B297" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="C295" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A296" s="5" t="s">
+      <c r="C297" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A298" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="B296" s="4" t="s">
+      <c r="B298" s="4" t="s">
         <v>614</v>
-      </c>
-      <c r="C296" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A297" s="8" t="s">
-        <v>617</v>
-      </c>
-      <c r="B297" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="C297" s="4" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A298" s="8" t="s">
-        <v>618</v>
-      </c>
-      <c r="B298" s="4" t="s">
-        <v>615</v>
       </c>
       <c r="C298" s="4" t="s">
         <v>613</v>
@@ -9420,7 +9445,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B299" s="4" t="s">
         <v>615</v>
@@ -9431,7 +9456,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" s="8" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B300" s="4" t="s">
         <v>615</v>
@@ -9442,7 +9467,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" s="8" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B301" s="4" t="s">
         <v>615</v>
@@ -9453,12 +9478,34 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" s="8" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B302" s="4" t="s">
         <v>615</v>
       </c>
       <c r="C302" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A303" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="B303" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C303" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A304" s="8" t="s">
+        <v>622</v>
+      </c>
+      <c r="B304" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C304" s="4" t="s">
         <v>613</v>
       </c>
     </row>
@@ -9469,17 +9516,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2854f1a0eb82b4299baec9a2bc5fa3aa">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e5d0997856646832757f031b0a9b789" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
     <xsd:import namespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
     <xsd:element name="properties">
@@ -9561,7 +9599,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -9582,7 +9620,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -9601,7 +9639,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -9618,8 +9656,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -9708,7 +9746,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
@@ -9718,16 +9756,17 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E67016B-2BB4-478C-AF15-1A9FF8562EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3851087F-07D3-4405-A433-7A0ADDCA2D10}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EABBD6-779A-48CC-9ED2-A26C957FCC1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -9745,7 +9784,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8338AF-8AC2-43D7-8F90-72D0B1807480}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9753,4 +9792,12 @@
     <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E67016B-2BB4-478C-AF15-1A9FF8562EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update model data with last model NZ6
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/B1_Model_Structure.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/B1_Model_Structure.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86724C66-F305-4FFC-AF3E-403D167AB920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{86724C66-F305-4FFC-AF3E-403D167AB920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52069E91-D434-4DA4-906D-136DA54D34FC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,8 +14,8 @@
     <sheet name="sector" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">sector!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sets!$A$3:$L$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">sector!$A$1:$D$293</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sets!$A$3:$L$295</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="622">
   <si>
     <t>set</t>
   </si>
@@ -1988,7 +1988,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2061,6 +2061,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -2126,7 +2132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2148,6 +2154,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2437,8 +2444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L295"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C278" sqref="C278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4768,6 +4775,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:L295" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -6187,9 +6195,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED10C39E-557A-4278-BB05-98C0EDA618C0}">
-  <dimension ref="A1:G282"/>
+  <dimension ref="A1:D293"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="A283" sqref="A283:A293"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6197,7 +6207,7 @@
     <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -7544,7 +7554,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>234</v>
       </c>
@@ -7558,7 +7568,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>236</v>
       </c>
@@ -7572,7 +7582,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>240</v>
       </c>
@@ -7586,7 +7596,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>242</v>
       </c>
@@ -7600,7 +7610,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>244</v>
       </c>
@@ -7614,7 +7624,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>246</v>
       </c>
@@ -7628,7 +7638,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>248</v>
       </c>
@@ -7642,7 +7652,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>250</v>
       </c>
@@ -7656,7 +7666,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>252</v>
       </c>
@@ -7669,9 +7679,8 @@
       <c r="D105" s="13" t="s">
         <v>603</v>
       </c>
-      <c r="G105" s="10"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>121</v>
       </c>
@@ -7685,7 +7694,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>123</v>
       </c>
@@ -7699,7 +7708,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>256</v>
       </c>
@@ -7713,7 +7722,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>258</v>
       </c>
@@ -7727,7 +7736,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>260</v>
       </c>
@@ -7741,7 +7750,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>262</v>
       </c>
@@ -7755,7 +7764,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>264</v>
       </c>
@@ -8889,7 +8898,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>416</v>
       </c>
@@ -8903,7 +8912,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="6" t="s">
         <v>417</v>
       </c>
@@ -8917,7 +8926,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="8" t="s">
         <v>418</v>
       </c>
@@ -8931,7 +8940,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="8" t="s">
         <v>419</v>
       </c>
@@ -8945,7 +8954,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="8" t="s">
         <v>420</v>
       </c>
@@ -8959,7 +8968,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="8" t="s">
         <v>424</v>
       </c>
@@ -8973,7 +8982,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="8" t="s">
         <v>425</v>
       </c>
@@ -8987,7 +8996,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="8" t="s">
         <v>421</v>
       </c>
@@ -9001,7 +9010,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="8" t="s">
         <v>422</v>
       </c>
@@ -9015,7 +9024,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="8" t="s">
         <v>423</v>
       </c>
@@ -9029,7 +9038,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="8" t="s">
         <v>426</v>
       </c>
@@ -9043,7 +9052,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="8" t="s">
         <v>427</v>
       </c>
@@ -9057,7 +9066,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="8" t="s">
         <v>428</v>
       </c>
@@ -9071,7 +9080,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="8" t="s">
         <v>429</v>
       </c>
@@ -9085,7 +9094,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="8" t="s">
         <v>430</v>
       </c>
@@ -9099,7 +9108,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="8" t="s">
         <v>431</v>
       </c>
@@ -9112,9 +9121,8 @@
       <c r="D208" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F208" s="10"/>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="8" t="s">
         <v>432</v>
       </c>
@@ -9127,9 +9135,8 @@
       <c r="D209" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F209" s="10"/>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="8" t="s">
         <v>433</v>
       </c>
@@ -9142,9 +9149,8 @@
       <c r="D210" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F210" s="10"/>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="8" t="s">
         <v>434</v>
       </c>
@@ -9157,9 +9163,8 @@
       <c r="D211" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F211" s="10"/>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="8" t="s">
         <v>435</v>
       </c>
@@ -9172,9 +9177,8 @@
       <c r="D212" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F212" s="10"/>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="8" t="s">
         <v>436</v>
       </c>
@@ -9187,9 +9191,8 @@
       <c r="D213" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F213" s="10"/>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="8" t="s">
         <v>437</v>
       </c>
@@ -9202,9 +9205,8 @@
       <c r="D214" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F214" s="10"/>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="8" t="s">
         <v>438</v>
       </c>
@@ -9217,9 +9219,8 @@
       <c r="D215" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F215" s="10"/>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="8" t="s">
         <v>439</v>
       </c>
@@ -9232,9 +9233,8 @@
       <c r="D216" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F216" s="10"/>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="8" t="s">
         <v>440</v>
       </c>
@@ -9247,9 +9247,8 @@
       <c r="D217" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F217" s="10"/>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="8" t="s">
         <v>441</v>
       </c>
@@ -9262,9 +9261,8 @@
       <c r="D218" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F218" s="10"/>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="8" t="s">
         <v>442</v>
       </c>
@@ -9277,9 +9275,8 @@
       <c r="D219" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F219" s="10"/>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="8" t="s">
         <v>443</v>
       </c>
@@ -9292,9 +9289,8 @@
       <c r="D220" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F220" s="10"/>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="8" t="s">
         <v>444</v>
       </c>
@@ -9307,9 +9303,8 @@
       <c r="D221" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F221" s="10"/>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="8" t="s">
         <v>445</v>
       </c>
@@ -9322,9 +9317,8 @@
       <c r="D222" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F222" s="10"/>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="8" t="s">
         <v>446</v>
       </c>
@@ -9337,9 +9331,8 @@
       <c r="D223" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F223" s="10"/>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="8" t="s">
         <v>447</v>
       </c>
@@ -9352,9 +9345,8 @@
       <c r="D224" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F224" s="10"/>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="8" t="s">
         <v>448</v>
       </c>
@@ -9367,9 +9359,8 @@
       <c r="D225" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F225" s="10"/>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="8" t="s">
         <v>449</v>
       </c>
@@ -9382,9 +9373,8 @@
       <c r="D226" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F226" s="10"/>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="8" t="s">
         <v>450</v>
       </c>
@@ -9397,9 +9387,8 @@
       <c r="D227" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F227" s="10"/>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="8" t="s">
         <v>451</v>
       </c>
@@ -9412,9 +9401,8 @@
       <c r="D228" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F228" s="10"/>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="8" t="s">
         <v>452</v>
       </c>
@@ -9427,9 +9415,8 @@
       <c r="D229" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F229" s="10"/>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="8" t="s">
         <v>453</v>
       </c>
@@ -9442,9 +9429,8 @@
       <c r="D230" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F230" s="10"/>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="8" t="s">
         <v>454</v>
       </c>
@@ -9457,9 +9443,8 @@
       <c r="D231" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F231" s="10"/>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="8" t="s">
         <v>455</v>
       </c>
@@ -9472,9 +9457,8 @@
       <c r="D232" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F232" s="10"/>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="8" t="s">
         <v>456</v>
       </c>
@@ -9487,9 +9471,8 @@
       <c r="D233" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F233" s="10"/>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="8" t="s">
         <v>457</v>
       </c>
@@ -9502,9 +9485,8 @@
       <c r="D234" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F234" s="10"/>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="8" t="s">
         <v>458</v>
       </c>
@@ -9517,9 +9499,8 @@
       <c r="D235" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F235" s="10"/>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="8" t="s">
         <v>459</v>
       </c>
@@ -9532,9 +9513,8 @@
       <c r="D236" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F236" s="10"/>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="8" t="s">
         <v>460</v>
       </c>
@@ -9547,9 +9527,8 @@
       <c r="D237" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F237" s="10"/>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="8" t="s">
         <v>461</v>
       </c>
@@ -9562,9 +9541,8 @@
       <c r="D238" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F238" s="10"/>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="8" t="s">
         <v>462</v>
       </c>
@@ -9577,9 +9555,8 @@
       <c r="D239" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F239" s="10"/>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="8" t="s">
         <v>463</v>
       </c>
@@ -9592,9 +9569,8 @@
       <c r="D240" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F240" s="10"/>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="8" t="s">
         <v>464</v>
       </c>
@@ -9607,9 +9583,8 @@
       <c r="D241" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F241" s="10"/>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="8" t="s">
         <v>465</v>
       </c>
@@ -9622,9 +9597,8 @@
       <c r="D242" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F242" s="10"/>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="8" t="s">
         <v>466</v>
       </c>
@@ -9637,9 +9611,8 @@
       <c r="D243" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F243" s="10"/>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="8" t="s">
         <v>467</v>
       </c>
@@ -9652,9 +9625,8 @@
       <c r="D244" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F244" s="10"/>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="8" t="s">
         <v>468</v>
       </c>
@@ -9667,9 +9639,8 @@
       <c r="D245" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F245" s="10"/>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="8" t="s">
         <v>469</v>
       </c>
@@ -9682,9 +9653,8 @@
       <c r="D246" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F246" s="10"/>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="8" t="s">
         <v>470</v>
       </c>
@@ -9697,9 +9667,8 @@
       <c r="D247" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F247" s="10"/>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="8" t="s">
         <v>471</v>
       </c>
@@ -9712,9 +9681,8 @@
       <c r="D248" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F248" s="10"/>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="8" t="s">
         <v>472</v>
       </c>
@@ -9727,9 +9695,8 @@
       <c r="D249" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F249" s="10"/>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="8" t="s">
         <v>473</v>
       </c>
@@ -9742,9 +9709,8 @@
       <c r="D250" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F250" s="10"/>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="8" t="s">
         <v>474</v>
       </c>
@@ -9757,9 +9723,8 @@
       <c r="D251" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F251" s="10"/>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="8" t="s">
         <v>475</v>
       </c>
@@ -9772,9 +9737,8 @@
       <c r="D252" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F252" s="10"/>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="8" t="s">
         <v>476</v>
       </c>
@@ -9787,9 +9751,8 @@
       <c r="D253" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F253" s="10"/>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="8" t="s">
         <v>477</v>
       </c>
@@ -9802,9 +9765,8 @@
       <c r="D254" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F254" s="10"/>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="8" t="s">
         <v>478</v>
       </c>
@@ -9817,9 +9779,8 @@
       <c r="D255" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F255" s="10"/>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="8" t="s">
         <v>479</v>
       </c>
@@ -9832,9 +9793,8 @@
       <c r="D256" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F256" s="10"/>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" s="8" t="s">
         <v>480</v>
       </c>
@@ -9847,9 +9807,8 @@
       <c r="D257" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F257" s="10"/>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="8" t="s">
         <v>481</v>
       </c>
@@ -9862,9 +9821,8 @@
       <c r="D258" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F258" s="10"/>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="8" t="s">
         <v>482</v>
       </c>
@@ -9877,9 +9835,8 @@
       <c r="D259" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F259" s="10"/>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="8" t="s">
         <v>483</v>
       </c>
@@ -9892,9 +9849,8 @@
       <c r="D260" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F260" s="10"/>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="8" t="s">
         <v>484</v>
       </c>
@@ -9907,9 +9863,8 @@
       <c r="D261" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F261" s="10"/>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="8" t="s">
         <v>485</v>
       </c>
@@ -9922,9 +9877,8 @@
       <c r="D262" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F262" s="10"/>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="8" t="s">
         <v>486</v>
       </c>
@@ -9937,9 +9891,8 @@
       <c r="D263" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F263" s="10"/>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="8" t="s">
         <v>487</v>
       </c>
@@ -9952,9 +9905,8 @@
       <c r="D264" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F264" s="10"/>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="8" t="s">
         <v>488</v>
       </c>
@@ -9967,9 +9919,8 @@
       <c r="D265" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F265" s="10"/>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="8" t="s">
         <v>489</v>
       </c>
@@ -9982,9 +9933,8 @@
       <c r="D266" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F266" s="10"/>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" s="8" t="s">
         <v>490</v>
       </c>
@@ -9997,9 +9947,8 @@
       <c r="D267" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F267" s="10"/>
-    </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="8" t="s">
         <v>491</v>
       </c>
@@ -10012,9 +9961,8 @@
       <c r="D268" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F268" s="10"/>
-    </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="8" t="s">
         <v>492</v>
       </c>
@@ -10027,9 +9975,8 @@
       <c r="D269" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F269" s="10"/>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" s="8" t="s">
         <v>493</v>
       </c>
@@ -10042,9 +9989,8 @@
       <c r="D270" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F270" s="10"/>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="8" t="s">
         <v>494</v>
       </c>
@@ -10057,9 +10003,8 @@
       <c r="D271" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F271" s="10"/>
-    </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="8" t="s">
         <v>495</v>
       </c>
@@ -10072,9 +10017,8 @@
       <c r="D272" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F272" s="10"/>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="8" t="s">
         <v>496</v>
       </c>
@@ -10087,9 +10031,8 @@
       <c r="D273" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F273" s="10"/>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="8" t="s">
         <v>497</v>
       </c>
@@ -10102,9 +10045,8 @@
       <c r="D274" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F274" s="10"/>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="8" t="s">
         <v>498</v>
       </c>
@@ -10117,10 +10059,9 @@
       <c r="D275" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F275" s="10"/>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A276" s="8" t="s">
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A276" s="21" t="s">
         <v>499</v>
       </c>
       <c r="B276" s="9" t="s">
@@ -10132,9 +10073,8 @@
       <c r="D276" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="F276" s="10"/>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277" s="5" t="s">
         <v>503</v>
       </c>
@@ -10148,7 +10088,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" s="5" t="s">
         <v>504</v>
       </c>
@@ -10162,7 +10102,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279" s="5" t="s">
         <v>505</v>
       </c>
@@ -10176,7 +10116,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280" s="5" t="s">
         <v>502</v>
       </c>
@@ -10190,7 +10130,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281" s="4" t="s">
         <v>500</v>
       </c>
@@ -10204,7 +10144,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282" s="4" t="s">
         <v>501</v>
       </c>
@@ -10218,33 +10158,168 @@
         <v>605</v>
       </c>
     </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A283" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B283" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C283" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D283" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A284" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C284" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D284" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A285" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B285" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C285" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D285" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A286" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="B286" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C286" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D286" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A287" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="B287" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C287" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D287" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A288" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="B288" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C288" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D288" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A289" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B289" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D289" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A290" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="B290" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C290" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D290" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A291" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B291" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D291" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A292" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="B292" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C292" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D292" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A293" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="B293" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D293" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D282" xr:uid="{51B380EC-F6E5-4369-BC41-BC40A47B4895}"/>
+  <autoFilter ref="A1:D293" xr:uid="{51B380EC-F6E5-4369-BC41-BC40A47B4895}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="694dc5982778b78571808a8a0bab1175">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac46d101c58d29857918b5bc3d6299d1" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -10475,14 +10550,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8338AF-8AC2-43D7-8F90-72D0B1807480}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{585148F4-AA9F-4384-93B2-8474BB8B5E18}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10494,5 +10582,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFBDF0BD-7BC3-494E-A10E-19C46C6B1FC8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8338AF-8AC2-43D7-8F90-72D0B1807480}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>